<commit_message>
fix: Arregla nomenclatura del cronograma
</commit_message>
<xml_diff>
--- a/02 DESARROLLO/DSEVI/01 Sprint 1/01 Planificación y Análisis/DSEVI-CP.xlsx
+++ b/02 DESARROLLO/DSEVI/01 Sprint 1/01 Planificación y Análisis/DSEVI-CP.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj3QCUXTk++yDpTJtvFoKzzZQC88w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjYTkJS/MtcLouSoeLKOGWPVCnavA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="112">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -24,7 +24,7 @@
     <t>Ruta del repositorio del proyecto:</t>
   </si>
   <si>
-    <t>https://github.com/isaacNull/Soft-Home.git</t>
+    <t>https://github.com/Garuel/SoftHome</t>
   </si>
   <si>
     <t>Grupo:</t>
@@ -54,6 +54,12 @@
     <t>David Villacis Alvear</t>
   </si>
   <si>
+    <t>Cuando son mismos documentos puede se : 
+DSEVI-ECU-01.docx, DSEVI-ECU-02.docx
+Si se repite Analisis o arquitectura 
+DSEVI-ARD.docx, DSEVI-AND.docx</t>
+  </si>
+  <si>
     <t>Actividad</t>
   </si>
   <si>
@@ -93,154 +99,259 @@
     <t>Project Charter</t>
   </si>
   <si>
+    <t>DSEVI-PC.docx</t>
+  </si>
+  <si>
+    <t>Leoncio</t>
+  </si>
+  <si>
     <t>Definir el cronograma del proyecto</t>
   </si>
   <si>
     <t>Cronograma</t>
   </si>
   <si>
+    <t>DSEVI-CP.xlsx</t>
+  </si>
+  <si>
+    <t>Jhon, Isaac</t>
+  </si>
+  <si>
     <t>Definir Historias de Usuarios</t>
   </si>
   <si>
+    <t xml:space="preserve">Documento de historias de usuario </t>
+  </si>
+  <si>
+    <t>DSEVI-HU.docx</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Crear y configurar el repositorio del proyecto</t>
+  </si>
+  <si>
+    <t>Repositorio GitHub</t>
+  </si>
+  <si>
+    <t>Isaac, Sebastian</t>
+  </si>
+  <si>
+    <t>DISEÑO</t>
+  </si>
+  <si>
+    <t>Semana 6</t>
+  </si>
+  <si>
+    <t>Prototipar las interfaces web del proyecto</t>
+  </si>
+  <si>
+    <t>Mockups y prototipos de las interfaces web</t>
+  </si>
+  <si>
+    <t>DSEVI-MPIW.docx</t>
+  </si>
+  <si>
+    <t>Jorge Armando</t>
+  </si>
+  <si>
+    <t>Diseñar la base de datos del proyecto</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de la Base de Datos</t>
+  </si>
+  <si>
+    <t>DSEVI-DEBD.docx</t>
+  </si>
+  <si>
+    <t>Diseñar la arquitectura del proyecto</t>
+  </si>
+  <si>
+    <t>Documento de Arquitectura del Software</t>
+  </si>
+  <si>
+    <t>DSEVI-DAS.docx</t>
+  </si>
+  <si>
+    <t>Paulo</t>
+  </si>
+  <si>
+    <t>Revisión y retrospecetiva de la fase de análisis y diseño</t>
+  </si>
+  <si>
+    <t>Reporte del sprint 1</t>
+  </si>
+  <si>
+    <t>DSEVI-RS1.docx</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>HITO 1</t>
+  </si>
+  <si>
+    <t>DESARROLLO</t>
+  </si>
+  <si>
+    <t>Semana 9</t>
+  </si>
+  <si>
+    <t>Desarrollar Página de incio</t>
+  </si>
+  <si>
+    <t>Módulo de página de inicio</t>
+  </si>
+  <si>
+    <t>pagina-inicio.html</t>
+  </si>
+  <si>
+    <t>Jhon, David</t>
+  </si>
+  <si>
+    <t>Desarrollar catálogo de videojuegos / bienes digitales</t>
+  </si>
+  <si>
+    <t>Módulo de catálogo</t>
+  </si>
+  <si>
+    <t>pagina-catalogo.html</t>
+  </si>
+  <si>
+    <t>Sebastian, David</t>
+  </si>
+  <si>
+    <t>Desarrollar sistema de compra</t>
+  </si>
+  <si>
+    <t>Módulo de Compra</t>
+  </si>
+  <si>
+    <t>pagina-compra.html</t>
+  </si>
+  <si>
+    <t>Sebastian, Isaac</t>
+  </si>
+  <si>
+    <t>Desarrollar sistema de donaciones</t>
+  </si>
+  <si>
+    <t>Módulo de donaciones</t>
+  </si>
+  <si>
+    <t>pagina-donaciones.html</t>
+  </si>
+  <si>
+    <t>David, Jorge</t>
+  </si>
+  <si>
+    <t>Desarrollar sección de comentarios</t>
+  </si>
+  <si>
+    <t>Módulo de comentarios</t>
+  </si>
+  <si>
+    <t>pagina-comentarios.html</t>
+  </si>
+  <si>
+    <t>Jhon, David, Jorge</t>
+  </si>
+  <si>
+    <t>Desarrollar autenticación de usuarios</t>
+  </si>
+  <si>
+    <t>Módulo de login</t>
+  </si>
+  <si>
+    <t>pagina-login.html</t>
+  </si>
+  <si>
+    <t>Desarrollar Dashboard</t>
+  </si>
+  <si>
+    <t>Módulo Dashboard</t>
+  </si>
+  <si>
+    <t>pagina-Dashboard.html</t>
+  </si>
+  <si>
+    <t>Revisión y retrospecetiva de la fase de desarrollo</t>
+  </si>
+  <si>
+    <t>Reporte del sprint 2</t>
+  </si>
+  <si>
+    <t>DSEVI-RS2.docx</t>
+  </si>
+  <si>
+    <t>HITO 2</t>
+  </si>
+  <si>
+    <t>PRUEBAS</t>
+  </si>
+  <si>
+    <t>Semana 10</t>
+  </si>
+  <si>
+    <t>Realizar pruebas de ambiente</t>
+  </si>
+  <si>
+    <t>Documento de Plan de Pruebas de Sotware</t>
+  </si>
+  <si>
+    <t>DSEVI-PPS.docx</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Realizar pruebas unitarias</t>
+  </si>
+  <si>
+    <t>DESPLIEGUE</t>
+  </si>
+  <si>
+    <t>Semana 11</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar las HU del Product Backlog</t>
+  </si>
+  <si>
     <t>Product Backlog</t>
   </si>
   <si>
-    <t>Crear y configurar el repositorio del proyecto</t>
-  </si>
-  <si>
-    <t>Repositorio GitHub</t>
-  </si>
-  <si>
-    <t>DISEÑO</t>
-  </si>
-  <si>
-    <t>Semana 6</t>
-  </si>
-  <si>
-    <t>Prototipar las interfaces web del proyecto</t>
-  </si>
-  <si>
-    <t>Mockups y prototipos de las interfaces web</t>
-  </si>
-  <si>
-    <t>Diseñar la base de datos del proyecto</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de la Base de Datos</t>
-  </si>
-  <si>
-    <t>Diseñar la arquitectura del proyecto</t>
-  </si>
-  <si>
-    <t>Documento de Arquitectura del Software</t>
-  </si>
-  <si>
-    <t>Revisión y retrospecetiva de la fase de análisis y diseño</t>
-  </si>
-  <si>
-    <t>Reporte del sprint 1</t>
-  </si>
-  <si>
-    <t>HITO 1</t>
-  </si>
-  <si>
-    <t>DESARROLLO</t>
-  </si>
-  <si>
-    <t>Semana 9</t>
-  </si>
-  <si>
-    <t>Desarrollar Página de incio</t>
-  </si>
-  <si>
-    <t>Módulo de página de inicio</t>
-  </si>
-  <si>
-    <t>Desarrollar catálogo de videojuegos / bienes digitales</t>
-  </si>
-  <si>
-    <t>Módulo de catálogo</t>
-  </si>
-  <si>
-    <t>Desarrollar sistema de compra</t>
-  </si>
-  <si>
-    <t>Módulo de Compra</t>
-  </si>
-  <si>
-    <t>Desarrollar sistema de donaciones</t>
-  </si>
-  <si>
-    <t>Módulo de donaciones</t>
-  </si>
-  <si>
-    <t>Desarrollar sección de comentarios</t>
-  </si>
-  <si>
-    <t>Módulo de comentarios</t>
-  </si>
-  <si>
-    <t>Desarrollar autenticación de usuarios</t>
-  </si>
-  <si>
-    <t>Módulo de login</t>
-  </si>
-  <si>
-    <t>Desarrollar Dashboard</t>
-  </si>
-  <si>
-    <t>Módulo Dashboard</t>
-  </si>
-  <si>
-    <t>Revisión y retrospecetiva de la fase de desarrollo</t>
-  </si>
-  <si>
-    <t>Reporte del sprint 2</t>
-  </si>
-  <si>
-    <t>HITO 2</t>
-  </si>
-  <si>
-    <t>PRUEBAS</t>
-  </si>
-  <si>
-    <t>Semana 10</t>
-  </si>
-  <si>
-    <t>Realizar pruebas de ambiente</t>
-  </si>
-  <si>
-    <t>Documento de Plan de Pruebas de Sotware</t>
-  </si>
-  <si>
-    <t>Realizar pruebas unitarias</t>
-  </si>
-  <si>
-    <t>DESPLIEGUE</t>
-  </si>
-  <si>
-    <t>Semana 11</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar las HU del Product Backlog</t>
+    <t>DSEVI-PB.docx</t>
   </si>
   <si>
     <t>Verificar y finalizar el diagrama de la base de datos</t>
   </si>
   <si>
+    <t>Isaac</t>
+  </si>
+  <si>
     <t>Verificar y finalizar la arquitectura de software y diseño de software</t>
   </si>
   <si>
+    <t>Jhon</t>
+  </si>
+  <si>
     <t>Realizar despliegue del proyecto</t>
   </si>
   <si>
     <t xml:space="preserve">Documento de plan de despliegue </t>
   </si>
   <si>
+    <t>DSEVI-PD.docx</t>
+  </si>
+  <si>
     <t>Revisión y retrospecetiva de la fase de pruebas y despliegue</t>
   </si>
   <si>
     <t>Reporte del sprint 3</t>
+  </si>
+  <si>
+    <t>DSEVI-RS3.docx</t>
   </si>
   <si>
     <t>HITO 3</t>
@@ -254,7 +365,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -264,6 +375,7 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -279,7 +391,7 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF0563C1"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -309,7 +421,22 @@
     </font>
     <font>
       <sz val="11.0"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -370,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border/>
     <border>
       <left/>
@@ -393,9 +520,11 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <bottom style="thin">
         <color rgb="FF000000"/>
-      </left>
+      </bottom>
+    </border>
+    <border>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -404,6 +533,14 @@
       </bottom>
     </border>
     <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -426,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -439,18 +576,31 @@
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -473,7 +623,10 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -484,37 +637,74 @@
     <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+    <xf borderId="3" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="7" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="6" fontId="10" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="6" fontId="11" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="6" fontId="12" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="7" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="11" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="2" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="2" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="6" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="15" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="15" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="13" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -857,679 +1047,771 @@
     </row>
     <row r="20">
       <c r="B20" s="1"/>
-      <c r="D20" s="8"/>
+      <c r="D20" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="C21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="D21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="F21" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="G21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="15" t="s">
+      <c r="H21" s="16" t="s">
         <v>19</v>
       </c>
+      <c r="I21" s="16" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="G22" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="22" t="s">
+      <c r="B23" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="24">
+      <c r="C23" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="27">
         <v>44818.0</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="27">
         <v>44825.0</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="28">
         <f t="shared" ref="H23:H26" si="1">G23-F23-INT((G23-F23-WEEKDAY(G23)+1)/7)</f>
         <v>7</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="29">
         <v>1.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="24">
+      <c r="B24" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="27">
         <v>44820.0</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="27">
         <v>44825.0</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="28">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="29">
         <v>1.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="24">
+      <c r="B25" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="27">
         <v>44825.0</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="27">
         <v>44832.0</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="28">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I25" s="27">
-        <v>0.0</v>
+      <c r="I25" s="33">
+        <v>1.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="24">
+      <c r="B26" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="27">
         <v>44823.0</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="27">
         <v>44827.0</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="28">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I26" s="26">
+      <c r="I26" s="29">
         <v>1.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="B27" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="24">
+      <c r="B28" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="27">
         <v>44841.0</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G28" s="27">
         <v>44846.0</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="28">
         <f t="shared" ref="H28:H31" si="2">G28-F28-INT((G28-F28-WEEKDAY(G28)+1)/7)</f>
         <v>5</v>
       </c>
-      <c r="I28" s="27">
-        <v>0.0</v>
+      <c r="I28" s="33">
+        <v>1.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="24">
+      <c r="B29" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="27">
         <v>44841.0</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="27">
         <v>44848.0</v>
       </c>
-      <c r="H29" s="25">
+      <c r="H29" s="28">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="24">
+      <c r="B30" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="27">
         <v>44842.0</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="27">
         <v>44850.0</v>
       </c>
-      <c r="H30" s="25">
+      <c r="H30" s="28">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I30" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="24">
+      <c r="B31" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="27">
         <v>44843.0</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="27">
         <v>44853.0</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="28">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="I31" s="27">
+      <c r="I31" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="33"/>
+      <c r="B32" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="41"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
+      <c r="B33" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="35">
+      <c r="B34" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="44">
         <v>44853.0</v>
       </c>
-      <c r="G34" s="35">
+      <c r="G34" s="44">
+        <v>44871.0</v>
+      </c>
+      <c r="H34" s="28">
+        <f t="shared" ref="H34:H41" si="3">G34-F34-INT((G34-F34-WEEKDAY(G34)+1)/7)</f>
+        <v>16</v>
+      </c>
+      <c r="I34" s="35">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="B35" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="44">
+        <v>44853.0</v>
+      </c>
+      <c r="G35" s="44">
+        <v>44871.0</v>
+      </c>
+      <c r="H35" s="28">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I35" s="35">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="B36" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="44">
         <v>44860.0</v>
       </c>
-      <c r="H34" s="25">
-        <f t="shared" ref="H34:H41" si="3">G34-F34-INT((G34-F34-WEEKDAY(G34)+1)/7)</f>
-        <v>7</v>
-      </c>
-      <c r="I34" s="27">
+      <c r="G36" s="44">
+        <v>44880.0</v>
+      </c>
+      <c r="H36" s="28">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="I36" s="35">
         <v>0.0</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="B35" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="35">
-        <v>44853.0</v>
-      </c>
-      <c r="G35" s="35">
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="B37" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="44">
         <v>44860.0</v>
       </c>
-      <c r="H35" s="25">
+      <c r="G37" s="44">
+        <v>44880.0</v>
+      </c>
+      <c r="H37" s="28">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I35" s="27">
+        <v>18</v>
+      </c>
+      <c r="I37" s="35">
         <v>0.0</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="35">
-        <v>44860.0</v>
-      </c>
-      <c r="G36" s="35">
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="B38" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="44">
         <v>44867.0</v>
       </c>
-      <c r="H36" s="25">
+      <c r="G38" s="44">
+        <v>44880.0</v>
+      </c>
+      <c r="H38" s="28">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I36" s="27">
+        <v>12</v>
+      </c>
+      <c r="I38" s="35">
         <v>0.0</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="34"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="35">
-        <v>44860.0</v>
-      </c>
-      <c r="G37" s="35">
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="B39" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="44">
         <v>44867.0</v>
       </c>
-      <c r="H37" s="25">
+      <c r="G39" s="44">
+        <v>44880.0</v>
+      </c>
+      <c r="H39" s="28">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I37" s="27">
+        <v>12</v>
+      </c>
+      <c r="I39" s="35">
         <v>0.0</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="34"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="35">
-        <v>44867.0</v>
-      </c>
-      <c r="G38" s="35">
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="B40" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="44">
         <v>44874.0</v>
       </c>
-      <c r="H38" s="25">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I38" s="27">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="B39" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="34"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="35">
-        <v>44867.0</v>
-      </c>
-      <c r="G39" s="35">
-        <v>44874.0</v>
-      </c>
-      <c r="H39" s="25">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I39" s="27">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="B40" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="34"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="35">
-        <v>44874.0</v>
-      </c>
-      <c r="G40" s="35">
+      <c r="G40" s="44">
         <v>44880.0</v>
       </c>
-      <c r="H40" s="25">
+      <c r="H40" s="28">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="I40" s="27">
+      <c r="I40" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="B41" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="35">
+      <c r="B41" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="44">
         <v>44880.0</v>
       </c>
-      <c r="G41" s="35">
+      <c r="G41" s="44">
         <v>44883.0</v>
       </c>
-      <c r="H41" s="25">
+      <c r="H41" s="28">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="I41" s="27">
+      <c r="I41" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="B42" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="33"/>
+      <c r="B42" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
+      <c r="B43" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="30"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="35">
+      <c r="B44" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" s="45">
         <v>44883.0</v>
       </c>
-      <c r="G44" s="35">
+      <c r="G44" s="45">
         <v>44885.0</v>
       </c>
-      <c r="H44" s="25">
+      <c r="H44" s="28">
         <f t="shared" ref="H44:H45" si="4">G44-F44-INT((G44-F44-WEEKDAY(G44)+1)/7)</f>
         <v>2</v>
       </c>
-      <c r="I44" s="27">
+      <c r="I44" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="B45" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="35">
+      <c r="B45" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F45" s="45">
         <v>44883.0</v>
       </c>
-      <c r="G45" s="35">
+      <c r="G45" s="45">
         <v>44885.0</v>
       </c>
-      <c r="H45" s="25">
+      <c r="H45" s="28">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="I45" s="27">
+      <c r="I45" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
+      <c r="B46" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="34"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="35">
+      <c r="B47" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F47" s="45">
         <v>44885.0</v>
       </c>
-      <c r="G47" s="35">
+      <c r="G47" s="45">
         <v>44890.0</v>
       </c>
-      <c r="H47" s="25">
+      <c r="H47" s="28">
         <f t="shared" ref="H47:H51" si="5">G47-F47-INT((G47-F47-WEEKDAY(G47)+1)/7)</f>
         <v>5</v>
       </c>
-      <c r="I47" s="27">
+      <c r="I47" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="34"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="35">
+      <c r="B48" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" s="45">
         <v>44885.0</v>
       </c>
-      <c r="G48" s="35">
+      <c r="G48" s="45">
         <v>44890.0</v>
       </c>
-      <c r="H48" s="25">
+      <c r="H48" s="28">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="I48" s="27">
+      <c r="I48" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D49" s="34"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="35">
+      <c r="B49" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="F49" s="45">
         <v>44885.0</v>
       </c>
-      <c r="G49" s="35">
+      <c r="G49" s="45">
         <v>44890.0</v>
       </c>
-      <c r="H49" s="25">
+      <c r="H49" s="28">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="I49" s="27">
+      <c r="I49" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="B50" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D50" s="34"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="35">
+      <c r="B50" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50" s="45">
         <v>44885.0</v>
       </c>
-      <c r="G50" s="35">
+      <c r="G50" s="45">
         <v>44890.0</v>
       </c>
-      <c r="H50" s="25">
+      <c r="H50" s="28">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="I50" s="27">
+      <c r="I50" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C51" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D51" s="34"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="35">
+      <c r="B51" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="E51" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" s="45">
         <v>44885.0</v>
       </c>
-      <c r="G51" s="35">
+      <c r="G51" s="45">
         <v>44890.0</v>
       </c>
-      <c r="H51" s="25">
+      <c r="H51" s="28">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="I51" s="27">
+      <c r="I51" s="35">
         <v>0.0</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="33"/>
+      <c r="B52" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="41"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="B53" s="1"/>

</xml_diff>

<commit_message>
Actualización de Cronograma (progreso)
</commit_message>
<xml_diff>
--- a/02 DESARROLLO/DSEVI/01 Sprint 1/01 Planificación y Análisis/DSEVI-CP.xlsx
+++ b/02 DESARROLLO/DSEVI/01 Sprint 1/01 Planificación y Análisis/DSEVI-CP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Desktop\DSEVI-ProyectoGC\SoftHome\02 DESARROLLO\DSEVI\01 Sprint 1\01 Planificación y Análisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAE188D-8F36-4CF1-8C76-379637D1627F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007F9A55-9BF8-4449-8B2D-15A7F6B276DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -676,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -771,9 +771,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1031,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1058,16 +1055,16 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:9" ht="30.6" customHeight="1">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
     </row>
     <row r="4" spans="2:9" ht="14.4">
       <c r="B4" s="1"/>
@@ -1270,7 +1267,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="50" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="29" t="s">
@@ -1297,7 +1294,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B26" s="52"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="29" t="s">
         <v>35</v>
       </c>
@@ -1322,7 +1319,7 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B27" s="52"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="33" t="s">
         <v>37</v>
       </c>
@@ -1347,7 +1344,7 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B28" s="52"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="33" t="s">
         <v>39</v>
       </c>
@@ -1372,7 +1369,7 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B29" s="52"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="33" t="s">
         <v>41</v>
       </c>
@@ -1397,7 +1394,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B30" s="52"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="33" t="s">
         <v>43</v>
       </c>
@@ -1422,7 +1419,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B31" s="53"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="29" t="s">
         <v>45</v>
       </c>
@@ -1564,21 +1561,21 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I36" s="37">
-        <v>0.6</v>
+      <c r="I36" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="39" t="s">
+      <c r="D37" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F37" s="26">
@@ -1591,21 +1588,21 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I37" s="44">
-        <v>0.8</v>
+      <c r="I37" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="56"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="55"/>
     </row>
     <row r="39" spans="2:9" ht="15.75" customHeight="1">
       <c r="B39" s="16" t="s">
@@ -1627,26 +1624,26 @@
       <c r="B40" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="42" t="s">
+      <c r="D40" s="41" t="s">
         <v>72</v>
       </c>
       <c r="E40" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="F40" s="43">
+      <c r="F40" s="42">
         <v>44853</v>
       </c>
-      <c r="G40" s="43">
+      <c r="G40" s="42">
         <v>44871</v>
       </c>
       <c r="H40" s="27">
         <f t="shared" ref="H40:H47" si="2">G40-F40-INT((G40-F40-WEEKDAY(G40)+1)/7)</f>
         <v>16</v>
       </c>
-      <c r="I40" s="44">
+      <c r="I40" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1654,26 +1651,26 @@
       <c r="B41" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="42" t="s">
+      <c r="D41" s="41" t="s">
         <v>76</v>
       </c>
       <c r="E41" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="F41" s="43">
+      <c r="F41" s="42">
         <v>44853</v>
       </c>
-      <c r="G41" s="43">
+      <c r="G41" s="42">
         <v>44871</v>
       </c>
       <c r="H41" s="27">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="I41" s="44">
+      <c r="I41" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1681,26 +1678,26 @@
       <c r="B42" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="42" t="s">
+      <c r="D42" s="41" t="s">
         <v>80</v>
       </c>
       <c r="E42" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="F42" s="43">
+      <c r="F42" s="42">
         <v>44860</v>
       </c>
-      <c r="G42" s="43">
+      <c r="G42" s="42">
         <v>44880</v>
       </c>
       <c r="H42" s="27">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="I42" s="44">
+      <c r="I42" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1708,26 +1705,26 @@
       <c r="B43" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C43" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="42" t="s">
+      <c r="D43" s="41" t="s">
         <v>84</v>
       </c>
       <c r="E43" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="F43" s="43">
+      <c r="F43" s="42">
         <v>44860</v>
       </c>
-      <c r="G43" s="43">
+      <c r="G43" s="42">
         <v>44880</v>
       </c>
       <c r="H43" s="27">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="I43" s="44">
+      <c r="I43" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1735,26 +1732,26 @@
       <c r="B44" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="41" t="s">
         <v>88</v>
       </c>
       <c r="E44" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="F44" s="43">
+      <c r="F44" s="42">
         <v>44867</v>
       </c>
-      <c r="G44" s="43">
+      <c r="G44" s="42">
         <v>44880</v>
       </c>
       <c r="H44" s="27">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="I44" s="44">
+      <c r="I44" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1762,26 +1759,26 @@
       <c r="B45" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="41" t="s">
         <v>92</v>
       </c>
       <c r="E45" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="F45" s="43">
+      <c r="F45" s="42">
         <v>44867</v>
       </c>
-      <c r="G45" s="43">
+      <c r="G45" s="42">
         <v>44880</v>
       </c>
       <c r="H45" s="27">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="I45" s="44">
+      <c r="I45" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1789,67 +1786,67 @@
       <c r="B46" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="41" t="s">
+      <c r="C46" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="D46" s="42" t="s">
+      <c r="D46" s="41" t="s">
         <v>95</v>
       </c>
       <c r="E46" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="43">
+      <c r="F46" s="42">
         <v>44874</v>
       </c>
-      <c r="G46" s="43">
+      <c r="G46" s="42">
         <v>44880</v>
       </c>
       <c r="H46" s="27">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="I46" s="44">
+      <c r="I46" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="39" t="s">
+      <c r="C47" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D47" s="39" t="s">
+      <c r="D47" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E47" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="43">
+      <c r="F47" s="42">
         <v>44880</v>
       </c>
-      <c r="G47" s="43">
+      <c r="G47" s="42">
         <v>44883</v>
       </c>
       <c r="H47" s="27">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="I47" s="44">
+      <c r="I47" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B48" s="54" t="s">
+      <c r="B48" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="56"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="55"/>
     </row>
     <row r="49" spans="2:9" ht="15.75" customHeight="1">
       <c r="B49" s="16" t="s">
@@ -1868,56 +1865,56 @@
       <c r="I49" s="21"/>
     </row>
     <row r="50" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B50" s="38" t="s">
+      <c r="B50" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="39" t="s">
+      <c r="C50" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="39" t="s">
+      <c r="D50" s="38" t="s">
         <v>104</v>
       </c>
       <c r="E50" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="F50" s="45">
+      <c r="F50" s="44">
         <v>44883</v>
       </c>
-      <c r="G50" s="45">
+      <c r="G50" s="44">
         <v>44885</v>
       </c>
       <c r="H50" s="27">
         <f t="shared" ref="H50:H51" si="3">G50-F50-INT((G50-F50-WEEKDAY(G50)+1)/7)</f>
         <v>2</v>
       </c>
-      <c r="I50" s="44">
+      <c r="I50" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="C51" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D51" s="39" t="s">
+      <c r="D51" s="38" t="s">
         <v>104</v>
       </c>
       <c r="E51" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="F51" s="45">
+      <c r="F51" s="44">
         <v>44883</v>
       </c>
-      <c r="G51" s="45">
+      <c r="G51" s="44">
         <v>44885</v>
       </c>
       <c r="H51" s="27">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I51" s="44">
+      <c r="I51" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1938,34 +1935,34 @@
       <c r="I52" s="21"/>
     </row>
     <row r="53" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B53" s="46" t="s">
+      <c r="B53" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="47" t="s">
+      <c r="C53" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="D53" s="48" t="s">
+      <c r="D53" s="47" t="s">
         <v>111</v>
       </c>
       <c r="E53" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="F53" s="45">
+      <c r="F53" s="44">
         <v>44885</v>
       </c>
-      <c r="G53" s="45">
+      <c r="G53" s="44">
         <v>44890</v>
       </c>
       <c r="H53" s="27">
         <f t="shared" ref="H53:H57" si="4">G53-F53-INT((G53-F53-WEEKDAY(G53)+1)/7)</f>
         <v>5</v>
       </c>
-      <c r="I53" s="44">
+      <c r="I53" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B54" s="46" t="s">
+      <c r="B54" s="45" t="s">
         <v>112</v>
       </c>
       <c r="C54" s="23" t="s">
@@ -1977,22 +1974,22 @@
       <c r="E54" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="F54" s="45">
+      <c r="F54" s="44">
         <v>44885</v>
       </c>
-      <c r="G54" s="45">
+      <c r="G54" s="44">
         <v>44890</v>
       </c>
       <c r="H54" s="27">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="I54" s="44">
+      <c r="I54" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="45" t="s">
         <v>114</v>
       </c>
       <c r="C55" s="23" t="s">
@@ -2001,88 +1998,88 @@
       <c r="D55" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E55" s="46" t="s">
+      <c r="E55" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="F55" s="45">
+      <c r="F55" s="44">
         <v>44885</v>
       </c>
-      <c r="G55" s="45">
+      <c r="G55" s="44">
         <v>44890</v>
       </c>
       <c r="H55" s="27">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="I55" s="44">
+      <c r="I55" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B56" s="46" t="s">
+      <c r="B56" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="47" t="s">
+      <c r="C56" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="47" t="s">
+      <c r="D56" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="46" t="s">
+      <c r="E56" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="45">
+      <c r="F56" s="44">
         <v>44885</v>
       </c>
-      <c r="G56" s="45">
+      <c r="G56" s="44">
         <v>44890</v>
       </c>
       <c r="H56" s="27">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="I56" s="44">
+      <c r="I56" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B57" s="46" t="s">
+      <c r="B57" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="C57" s="47" t="s">
+      <c r="C57" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="39" t="s">
+      <c r="D57" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="E57" s="40" t="s">
+      <c r="E57" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F57" s="45">
+      <c r="F57" s="44">
         <v>44885</v>
       </c>
-      <c r="G57" s="45">
+      <c r="G57" s="44">
         <v>44890</v>
       </c>
       <c r="H57" s="27">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="I57" s="44">
+      <c r="I57" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B58" s="54" t="s">
+      <c r="B58" s="53" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="55"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="55"/>
-      <c r="H58" s="55"/>
-      <c r="I58" s="56"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="54"/>
+      <c r="I58" s="55"/>
     </row>
     <row r="59" spans="2:9" ht="15.75" customHeight="1">
       <c r="B59" s="1"/>

</xml_diff>